<commit_message>
Primarily work on courses.py
</commit_message>
<xml_diff>
--- a/TESTDATA/testing/FACHWAHL/Fachwahl_13.xlsx
+++ b/TESTDATA/testing/FACHWAHL/Fachwahl_13.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
-  <si>
-    <t xml:space="preserve">#</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t xml:space="preserve">Fächerwahl</t>
   </si>
@@ -446,10 +443,10 @@
   <dimension ref="A1:S1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.74"/>
@@ -461,16 +458,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -488,18 +483,18 @@
     </row>
     <row r="2" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -517,13 +512,13 @@
     </row>
     <row r="3" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -545,47 +540,47 @@
     <row r="4" customFormat="false" ht="8.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="44.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="10" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>11</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="L5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="M5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="N5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="O5" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>22</v>
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
@@ -594,43 +589,43 @@
     </row>
     <row r="6" customFormat="false" ht="94.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="11"/>
       <c r="E6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="G6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="J6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="K6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="L6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="M6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="N6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="O6" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>34</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -660,31 +655,31 @@
     </row>
     <row r="8" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="C8" s="16" t="s">
         <v>36</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>37</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
       <c r="O8" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P8" s="17"/>
       <c r="Q8" s="17"/>
@@ -693,18 +688,18 @@
     </row>
     <row r="9" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>40</v>
-      </c>
       <c r="C9" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
@@ -712,12 +707,12 @@
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
       <c r="O9" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P9" s="17"/>
       <c r="Q9" s="17"/>
@@ -726,30 +721,30 @@
     </row>
     <row r="10" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>42</v>
-      </c>
       <c r="C10" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10" s="17"/>
       <c r="J10" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
       <c r="N10" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
@@ -759,29 +754,29 @@
     </row>
     <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>44</v>
-      </c>
       <c r="C11" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
       <c r="M11" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N11" s="17"/>
       <c r="O11" s="17"/>
@@ -792,18 +787,18 @@
     </row>
     <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>46</v>
-      </c>
       <c r="C12" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -811,11 +806,11 @@
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M12" s="17"/>
       <c r="N12" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
@@ -864,7 +859,6 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <sheetProtection sheet="true"/>
   <mergeCells count="7">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:S1"/>

</xml_diff>